<commit_message>
Added BOM and notes needed for mechanical build of project to BuggyBOM.xlsx.
</commit_message>
<xml_diff>
--- a/RPi Buggy/Design Documentation/BuggyBOM.xlsx
+++ b/RPi Buggy/Design Documentation/BuggyBOM.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Documents\RPi Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Documents\RepoData\EmbeddedProjects\RPi Buggy\Design Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7939CC5-B62C-43AE-A60A-ABC41584D2AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB6A24A-9DE1-45B2-9723-89C78A9D4AD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{F8E2037D-8D84-4045-A7CE-8E5633B7B6C0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{F8E2037D-8D84-4045-A7CE-8E5633B7B6C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Electronics" sheetId="1" r:id="rId1"/>
     <sheet name="Motors + Wheels" sheetId="2" r:id="rId2"/>
+    <sheet name="Mechanical" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="98">
   <si>
     <t>Component</t>
   </si>
@@ -272,6 +273,107 @@
   </si>
   <si>
     <t>https://www.adafruit.com/product/1954</t>
+  </si>
+  <si>
+    <t>Build of Material for RPi Buggy (Electronics)
+Author: Edward Martinez
+Date: 03/20/2021
+Rev 1.0</t>
+  </si>
+  <si>
+    <t>Machine / stainless steel</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>Usage</t>
+  </si>
+  <si>
+    <t>Motor mount</t>
+  </si>
+  <si>
+    <t>Lowe's/HD/Hardware store</t>
+  </si>
+  <si>
+    <t>Caster wheel mount</t>
+  </si>
+  <si>
+    <t>*Note: round or oval bolts may be used instead of flats, but may limit usable surface area on the main body of the buggy</t>
+  </si>
+  <si>
+    <t>Main body</t>
+  </si>
+  <si>
+    <t>https://www.lowes.com/pd/OPTIX-0-08-in-T-x-8-in-W-x-10-in-L-Clear-Acrylic-Sheet/3143395</t>
+  </si>
+  <si>
+    <t>Lowe's</t>
+  </si>
+  <si>
+    <t>https://www.lowes.com/pd/Hillman-2-in-Wood-to-Wood-Silver-Triple-Zinc-Angle-3-Pack/3478179</t>
+  </si>
+  <si>
+    <t>*Angle brackets Note:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P/N listed allows for a single mounting point with the bracket due to location of slots.
+It is advisable to use a slightly longer bracket and drilling custom holes for #4 bolts.
+0.5'' is the maximum advisable dimension in the "vertical" axis, as any longer will interfere with the output shaft of the motor. See locations of motor mounting points in the link in the "Motors + Wheels" tab (3mm holes in drawing, use the #4 bolts listed)
+Suggested dimensions: 2.25-2.5'' x  0.5'' x ~3/8'' </t>
+  </si>
+  <si>
+    <t>Bracket to main body
+Note: shims need if using 0.5'', 1/4-3/8'' may work as well</t>
+  </si>
+  <si>
+    <t>Polycarbonate/Acryclic/plexiglass is fine. Thickness used here will drive thickness req'd for #6 bolts
+Can use larger/thicker sheet for greater payload capacity.</t>
+  </si>
+  <si>
+    <t>Hillman slotted angle bracket(1/2'' x 0.5'' x 2'' )</t>
+  </si>
+  <si>
+    <t>Optix/Plaskolite 8'' x 10'' x 0.080'' Acrylic sheet</t>
+  </si>
+  <si>
+    <t>Machine/zinc
+14 pcs</t>
+  </si>
+  <si>
+    <t>https://www.lowes.com/pd/Hillman-4-40-x-1-2-in-Slotted-Drive-Machine-Screws-14-Count/3036681</t>
+  </si>
+  <si>
+    <t>Hillman #4 - 40 x 1'' Flat Phillips bolts + nuts or equivalent</t>
+  </si>
+  <si>
+    <t>Machine / stainless steel
+=&gt; 0.5'' length will impede motion of the caster wheel
+14 pcs</t>
+  </si>
+  <si>
+    <t>https://www.lowes.com/pd/Hillman-6-32-x-3-8-in-Slotted-Drive-Machine-Screws-14-Count/3036684</t>
+  </si>
+  <si>
+    <t>Hillman #6 - 32 x 1/4-3/8'' Flat phillips bolts + nuts or equivalent</t>
+  </si>
+  <si>
+    <t>Everbilt #6 - 32 x 1/2'' Flat phillips bolts  + nuts or equivalent</t>
+  </si>
+  <si>
+    <t>Home Depot</t>
+  </si>
+  <si>
+    <t>https://www.homedepot.com/p/Everbilt-6-32-x-1-2-in-Phillips-Flat-Head-Zinc-Plated-Machine-Screw-8-Pack-803681/204274657
+https://www.homedepot.com/p/Everbilt-6-32-x-3-8-in-Phillips-Flat-Head-Brass-Machine-Screw-6-Pack-804271/204791323</t>
+  </si>
+  <si>
+    <t>Machine / stainless steel
+8pcs</t>
+  </si>
+  <si>
+    <t>Mounting point for motors
+2pcs</t>
   </si>
 </sst>
 </file>
@@ -349,7 +451,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -380,13 +482,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="20">
     <dxf>
       <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
       <fill>
@@ -423,6 +528,61 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -517,7 +677,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8A281FC4-C308-4A19-89A2-0B27B84F0E64}" name="Table1" displayName="Table1" ref="A4:I19" totalsRowCount="1" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8A281FC4-C308-4A19-89A2-0B27B84F0E64}" name="Table1" displayName="Table1" ref="A4:I19" totalsRowCount="1" headerRowDxfId="19">
   <autoFilter ref="A4:I18" xr:uid="{60A08667-E64D-424D-9AB0-346C0E96E253}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{B58CF5F9-CD9B-4A20-9151-1851A598F8E7}" name="_x000a_" totalsRowLabel="Total"/>
@@ -525,10 +685,10 @@
     <tableColumn id="3" xr3:uid="{2CB8C685-7066-4D11-B556-B7584EFBEE8E}" name="Vendor"/>
     <tableColumn id="4" xr3:uid="{A67F3285-2642-4C49-A851-6183D5A0547F}" name="P/N"/>
     <tableColumn id="5" xr3:uid="{DAD56C0D-5728-4CA2-A684-326242D1ECDE}" name="Price/unit" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{F43AF0D5-AD4E-42F3-A212-690E5B7AAD60}" name="Specs" dataDxfId="12" totalsRowDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{21C5FD30-037C-45BE-A44F-A87EBA50CAB2}" name="Link" totalsRowDxfId="10" dataCellStyle="Hyperlink"/>
-    <tableColumn id="8" xr3:uid="{CC4E6B6E-45C6-498B-923D-C834C9BBF83C}" name="Qty" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{531ED078-CA47-4810-A118-14D456877593}" name="Part Cost" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6">
+    <tableColumn id="6" xr3:uid="{F43AF0D5-AD4E-42F3-A212-690E5B7AAD60}" name="Specs" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{21C5FD30-037C-45BE-A44F-A87EBA50CAB2}" name="Link" totalsRowDxfId="16" dataCellStyle="Hyperlink"/>
+    <tableColumn id="8" xr3:uid="{CC4E6B6E-45C6-498B-923D-C834C9BBF83C}" name="Qty" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{531ED078-CA47-4810-A118-14D456877593}" name="Part Cost" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12">
       <calculatedColumnFormula>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Qty]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -537,7 +697,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2AB83441-1142-4B18-B5DC-A6B5B7673001}" name="Table4" displayName="Table4" ref="A2:I7" totalsRowCount="1" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2AB83441-1142-4B18-B5DC-A6B5B7673001}" name="Table4" displayName="Table4" ref="A2:I7" totalsRowCount="1" headerRowDxfId="11">
   <autoFilter ref="A2:I6" xr:uid="{961F1EFC-47C8-41AF-99D5-18F4498998C1}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{6A91A136-7421-429F-AC88-F3E8197C6CF9}" name="No." totalsRowLabel="Total"/>
@@ -546,13 +706,34 @@
     <tableColumn id="4" xr3:uid="{2ADFFBCA-067B-49B8-AA1B-2F7D293740BA}" name="P/N"/>
     <tableColumn id="5" xr3:uid="{7FBA3697-3048-4CCD-9FD8-F18E1CD3323F}" name="Price/unit"/>
     <tableColumn id="6" xr3:uid="{CA5B609A-7F2B-4636-AFDC-22533853B9FA}" name="Specs"/>
-    <tableColumn id="7" xr3:uid="{026D9F9F-A709-4C1F-A9A7-4BBCD7BDA398}" name="Link" totalsRowDxfId="2" dataCellStyle="Hyperlink"/>
-    <tableColumn id="8" xr3:uid="{0A0C0A78-F16F-4CE1-B6CE-9601146D83C1}" name="Qty" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="1" dataCellStyle="Currency"/>
-    <tableColumn id="9" xr3:uid="{E8467AE3-8A65-497D-AF64-A0236A1A3B32}" name="Cost" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="0" dataCellStyle="Currency">
+    <tableColumn id="7" xr3:uid="{026D9F9F-A709-4C1F-A9A7-4BBCD7BDA398}" name="Link" totalsRowDxfId="10" dataCellStyle="Hyperlink"/>
+    <tableColumn id="8" xr3:uid="{0A0C0A78-F16F-4CE1-B6CE-9601146D83C1}" name="Qty" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8" dataCellStyle="Currency"/>
+    <tableColumn id="9" xr3:uid="{E8467AE3-8A65-497D-AF64-A0236A1A3B32}" name="Cost" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6" dataCellStyle="Currency">
       <calculatedColumnFormula>Table4[[#This Row],[Price/unit]]*Table4[[#This Row],[Qty]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A9E0B485-5618-4773-9510-8DD45A7C266C}" name="Table43" displayName="Table43" ref="A2:J8" totalsRowCount="1" headerRowDxfId="5">
+  <autoFilter ref="A2:J7" xr:uid="{BDDF5B27-FBC8-42BF-8A48-800B14B0B8A0}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{445384C4-ABF7-4C30-8894-7C0E689C4B29}" name="No." totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{597CE3D1-88C9-4627-87D0-ABBB6C3CBB3B}" name="Component"/>
+    <tableColumn id="3" xr3:uid="{0B592AE4-41C3-4454-B802-29E2FDA8741B}" name="Vendor"/>
+    <tableColumn id="4" xr3:uid="{9DC898CD-D137-4124-A0D9-A67B27AD47C7}" name="P/N"/>
+    <tableColumn id="5" xr3:uid="{582B6AF6-E3B8-4D78-9F77-2A93E3E0EF85}" name="Price/unit"/>
+    <tableColumn id="6" xr3:uid="{A6547B14-5C53-419E-8211-C30D723A0205}" name="Specs"/>
+    <tableColumn id="10" xr3:uid="{9512E85F-6690-4EC4-A8D0-C52686B09DB2}" name="Usage"/>
+    <tableColumn id="7" xr3:uid="{25C45DF8-69BD-4369-922B-EEDD45F0F24D}" name="link" totalsRowDxfId="2" dataCellStyle="Hyperlink"/>
+    <tableColumn id="8" xr3:uid="{EBB86E6C-D04A-407D-B489-9469292F25EC}" name="Qty" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="1" dataCellStyle="Currency"/>
+    <tableColumn id="9" xr3:uid="{1E99713F-843C-4769-8034-B4A3CDACCE33}" name="Cost" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="0" dataCellStyle="Currency">
+      <calculatedColumnFormula>Table43[[#This Row],[Price/unit]]*Table43[[#This Row],[Qty]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -855,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC8A2087-E115-4C04-A572-A6D99C71BDF0}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1362,7 +1543,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1555,4 +1736,269 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E71F0255-F518-4C33-8379-619E3ECE9F60}">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="67.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.42578125" customWidth="1"/>
+    <col min="7" max="7" width="53" customWidth="1"/>
+    <col min="8" max="8" width="87.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="105" x14ac:dyDescent="0.35">
+      <c r="B1" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3">
+        <v>62179</v>
+      </c>
+      <c r="E3">
+        <v>1.28</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I3" s="12">
+        <v>1</v>
+      </c>
+      <c r="J3" s="13">
+        <f>Table43[[#This Row],[Price/unit]]*Table43[[#This Row],[Qty]]</f>
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4">
+        <v>491323</v>
+      </c>
+      <c r="E4">
+        <v>1.28</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I4" s="12">
+        <v>1</v>
+      </c>
+      <c r="J4" s="13">
+        <f>Table43[[#This Row],[Price/unit]]*Table43[[#This Row],[Qty]]</f>
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5">
+        <v>804271</v>
+      </c>
+      <c r="E5">
+        <v>1.18</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="I5" s="12">
+        <v>1</v>
+      </c>
+      <c r="J5" s="13">
+        <f>Table43[[#This Row],[Price/unit]]*Table43[[#This Row],[Qty]]</f>
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6">
+        <v>884489</v>
+      </c>
+      <c r="E6">
+        <v>1.87</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I6" s="12">
+        <v>2</v>
+      </c>
+      <c r="J6" s="13">
+        <f>Table43[[#This Row],[Price/unit]]*Table43[[#This Row],[Qty]]</f>
+        <v>3.74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7">
+        <v>55844</v>
+      </c>
+      <c r="E7">
+        <v>3.98</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" s="12">
+        <v>2</v>
+      </c>
+      <c r="J7" s="13">
+        <f>Table43[[#This Row],[Price/unit]]*Table43[[#This Row],[Qty]]</f>
+        <v>7.96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="I8" s="11">
+        <f>SUBTOTAL(109,Table43[Qty])</f>
+        <v>7</v>
+      </c>
+      <c r="J8" s="10">
+        <f>SUBTOTAL(109,Table43[Cost])</f>
+        <v>15.440000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H7" r:id="rId1" xr:uid="{4DF8F076-863C-4413-953A-0C2AECBC2379}"/>
+    <hyperlink ref="H6" r:id="rId2" xr:uid="{B42F1589-779D-424B-A4BA-E19D57A9AC0A}"/>
+    <hyperlink ref="H3" r:id="rId3" xr:uid="{347B1079-24CE-4036-A90A-509C81173316}"/>
+    <hyperlink ref="H4" r:id="rId4" xr:uid="{DE06405D-0DFD-4B54-9A35-5D58027D1386}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+  <tableParts count="1">
+    <tablePart r:id="rId6"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Electronics BOM with additional purchases and updated readme formatting.
</commit_message>
<xml_diff>
--- a/RPi Buggy/Design Documentation/BuggyBOM.xlsx
+++ b/RPi Buggy/Design Documentation/BuggyBOM.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Documents\RepoData\EmbeddedProjects\RPi Buggy\Design Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB6A24A-9DE1-45B2-9723-89C78A9D4AD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427EB553-E8B0-4A07-AA7F-C27C2A9E3D91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{F8E2037D-8D84-4045-A7CE-8E5633B7B6C0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{F8E2037D-8D84-4045-A7CE-8E5633B7B6C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Electronics" sheetId="1" r:id="rId1"/>
-    <sheet name="Motors + Wheels" sheetId="2" r:id="rId2"/>
-    <sheet name="Mechanical" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="Motors + Wheels" sheetId="2" r:id="rId3"/>
+    <sheet name="Mechanical" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="117">
   <si>
     <t>Component</t>
   </si>
@@ -114,9 +115,6 @@
   <si>
     <t>DC Jack connector
 8'' power cable</t>
-  </si>
-  <si>
-    <t>5V Powerboost</t>
   </si>
   <si>
     <t>500mA from 1.8V
@@ -374,6 +372,75 @@
   <si>
     <t>Mounting point for motors
 2pcs</t>
+  </si>
+  <si>
+    <t>PowerBoost 1000</t>
+  </si>
+  <si>
+    <t>PowerBoost 500</t>
+  </si>
+  <si>
+    <t>4A limit</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/2030</t>
+  </si>
+  <si>
+    <t>5V/3A buck regulator</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>LM2596S-5.0</t>
+  </si>
+  <si>
+    <t>Step-down, fixed output
+5V out, 3A max</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/LM2596S-5-0/3701226</t>
+  </si>
+  <si>
+    <t>MUX/DEMUX 8x1 16DIP</t>
+  </si>
+  <si>
+    <t>CD74HC4061E</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/CD74HC4051E/475938</t>
+  </si>
+  <si>
+    <t>MUX/DEMUX 8:1
+Preserve those precious Rpi GPIOs</t>
+  </si>
+  <si>
+    <t>Ultrasonic Distance Sensor</t>
+  </si>
+  <si>
+    <t>3V or 5V compatible</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/4007</t>
+  </si>
+  <si>
+    <t>9-DOF Accel/Mag/Gyro + Temp Breakout Board</t>
+  </si>
+  <si>
+    <t>Ranges:
++/- 2/4/6/8/16 g
++/- 2/4/8/12 gauss
++/- 245/500/2000 dps
+I2C or SPI interfaces</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/3387</t>
+  </si>
+  <si>
+    <t>Build of Material for RPi Buggy (Electronics)
+Author: Edward Martinez
+Date: 01/24/2021
+Rev 1.1</t>
   </si>
 </sst>
 </file>
@@ -502,7 +569,7 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -523,11 +590,44 @@
       </font>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -604,42 +704,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="10"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -677,18 +744,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8A281FC4-C308-4A19-89A2-0B27B84F0E64}" name="Table1" displayName="Table1" ref="A4:I19" totalsRowCount="1" headerRowDxfId="19">
-  <autoFilter ref="A4:I18" xr:uid="{60A08667-E64D-424D-9AB0-346C0E96E253}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8A281FC4-C308-4A19-89A2-0B27B84F0E64}" name="Table1" displayName="Table1" ref="A4:I24" totalsRowCount="1" headerRowDxfId="19">
+  <autoFilter ref="A4:I23" xr:uid="{60A08667-E64D-424D-9AB0-346C0E96E253}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{B58CF5F9-CD9B-4A20-9151-1851A598F8E7}" name="_x000a_" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{F108067D-FD63-4C90-84D1-70D71A784980}" name="Component"/>
     <tableColumn id="3" xr3:uid="{2CB8C685-7066-4D11-B556-B7584EFBEE8E}" name="Vendor"/>
     <tableColumn id="4" xr3:uid="{A67F3285-2642-4C49-A851-6183D5A0547F}" name="P/N"/>
     <tableColumn id="5" xr3:uid="{DAD56C0D-5728-4CA2-A684-326242D1ECDE}" name="Price/unit" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{F43AF0D5-AD4E-42F3-A212-690E5B7AAD60}" name="Specs" dataDxfId="18" totalsRowDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{21C5FD30-037C-45BE-A44F-A87EBA50CAB2}" name="Link" totalsRowDxfId="16" dataCellStyle="Hyperlink"/>
-    <tableColumn id="8" xr3:uid="{CC4E6B6E-45C6-498B-923D-C834C9BBF83C}" name="Qty" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{531ED078-CA47-4810-A118-14D456877593}" name="Part Cost" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12">
+    <tableColumn id="6" xr3:uid="{F43AF0D5-AD4E-42F3-A212-690E5B7AAD60}" name="Specs" dataDxfId="18" totalsRowDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{21C5FD30-037C-45BE-A44F-A87EBA50CAB2}" name="Link" totalsRowDxfId="2" dataCellStyle="Hyperlink"/>
+    <tableColumn id="8" xr3:uid="{CC4E6B6E-45C6-498B-923D-C834C9BBF83C}" name="Qty" totalsRowFunction="sum" dataDxfId="17" totalsRowDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{531ED078-CA47-4810-A118-14D456877593}" name="Part Cost" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="0">
       <calculatedColumnFormula>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Qty]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -697,7 +764,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2AB83441-1142-4B18-B5DC-A6B5B7673001}" name="Table4" displayName="Table4" ref="A2:I7" totalsRowCount="1" headerRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2AB83441-1142-4B18-B5DC-A6B5B7673001}" name="Table4" displayName="Table4" ref="A2:I7" totalsRowCount="1" headerRowDxfId="15">
   <autoFilter ref="A2:I6" xr:uid="{961F1EFC-47C8-41AF-99D5-18F4498998C1}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{6A91A136-7421-429F-AC88-F3E8197C6CF9}" name="No." totalsRowLabel="Total"/>
@@ -706,9 +773,9 @@
     <tableColumn id="4" xr3:uid="{2ADFFBCA-067B-49B8-AA1B-2F7D293740BA}" name="P/N"/>
     <tableColumn id="5" xr3:uid="{7FBA3697-3048-4CCD-9FD8-F18E1CD3323F}" name="Price/unit"/>
     <tableColumn id="6" xr3:uid="{CA5B609A-7F2B-4636-AFDC-22533853B9FA}" name="Specs"/>
-    <tableColumn id="7" xr3:uid="{026D9F9F-A709-4C1F-A9A7-4BBCD7BDA398}" name="Link" totalsRowDxfId="10" dataCellStyle="Hyperlink"/>
-    <tableColumn id="8" xr3:uid="{0A0C0A78-F16F-4CE1-B6CE-9601146D83C1}" name="Qty" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8" dataCellStyle="Currency"/>
-    <tableColumn id="9" xr3:uid="{E8467AE3-8A65-497D-AF64-A0236A1A3B32}" name="Cost" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6" dataCellStyle="Currency">
+    <tableColumn id="7" xr3:uid="{026D9F9F-A709-4C1F-A9A7-4BBCD7BDA398}" name="Link" totalsRowDxfId="14" dataCellStyle="Hyperlink"/>
+    <tableColumn id="8" xr3:uid="{0A0C0A78-F16F-4CE1-B6CE-9601146D83C1}" name="Qty" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12" dataCellStyle="Currency"/>
+    <tableColumn id="9" xr3:uid="{E8467AE3-8A65-497D-AF64-A0236A1A3B32}" name="Cost" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="10" dataCellStyle="Currency">
       <calculatedColumnFormula>Table4[[#This Row],[Price/unit]]*Table4[[#This Row],[Qty]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -717,7 +784,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A9E0B485-5618-4773-9510-8DD45A7C266C}" name="Table43" displayName="Table43" ref="A2:J8" totalsRowCount="1" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A9E0B485-5618-4773-9510-8DD45A7C266C}" name="Table43" displayName="Table43" ref="A2:J8" totalsRowCount="1" headerRowDxfId="9">
   <autoFilter ref="A2:J7" xr:uid="{BDDF5B27-FBC8-42BF-8A48-800B14B0B8A0}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{445384C4-ABF7-4C30-8894-7C0E689C4B29}" name="No." totalsRowLabel="Total"/>
@@ -727,9 +794,9 @@
     <tableColumn id="5" xr3:uid="{582B6AF6-E3B8-4D78-9F77-2A93E3E0EF85}" name="Price/unit"/>
     <tableColumn id="6" xr3:uid="{A6547B14-5C53-419E-8211-C30D723A0205}" name="Specs"/>
     <tableColumn id="10" xr3:uid="{9512E85F-6690-4EC4-A8D0-C52686B09DB2}" name="Usage"/>
-    <tableColumn id="7" xr3:uid="{25C45DF8-69BD-4369-922B-EEDD45F0F24D}" name="link" totalsRowDxfId="2" dataCellStyle="Hyperlink"/>
-    <tableColumn id="8" xr3:uid="{EBB86E6C-D04A-407D-B489-9469292F25EC}" name="Qty" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="1" dataCellStyle="Currency"/>
-    <tableColumn id="9" xr3:uid="{1E99713F-843C-4769-8034-B4A3CDACCE33}" name="Cost" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="0" dataCellStyle="Currency">
+    <tableColumn id="7" xr3:uid="{25C45DF8-69BD-4369-922B-EEDD45F0F24D}" name="link" totalsRowDxfId="8" dataCellStyle="Hyperlink"/>
+    <tableColumn id="8" xr3:uid="{EBB86E6C-D04A-407D-B489-9469292F25EC}" name="Qty" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6" dataCellStyle="Currency"/>
+    <tableColumn id="9" xr3:uid="{1E99713F-843C-4769-8034-B4A3CDACCE33}" name="Cost" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="4" dataCellStyle="Currency">
       <calculatedColumnFormula>Table43[[#This Row],[Price/unit]]*Table43[[#This Row],[Qty]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1034,10 +1101,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC8A2087-E115-4C04-A572-A6D99C71BDF0}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1055,15 +1122,15 @@
   <sheetData>
     <row r="1" spans="1:11" ht="84" x14ac:dyDescent="0.35">
       <c r="B1" s="15" t="s">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>0</v>
@@ -1084,10 +1151,10 @@
         <v>3</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1203,11 +1270,11 @@
         <v>14</v>
       </c>
       <c r="H8" s="8">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I8" s="5">
         <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Qty]]</f>
-        <v>9.5</v>
+        <v>2.8499999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1227,7 +1294,7 @@
         <v>20</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H9" s="8">
         <v>1</v>
@@ -1269,7 +1336,7 @@
     </row>
     <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -1281,7 +1348,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="8">
@@ -1297,7 +1364,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -1309,17 +1376,17 @@
         <v>9.9499999999999993</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="H12" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I12" s="5">
         <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Qty]]</f>
-        <v>19.899999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="105" x14ac:dyDescent="0.25">
@@ -1327,7 +1394,7 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -1339,10 +1406,10 @@
         <v>7.5</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="H13" s="8">
         <v>3</v>
@@ -1357,7 +1424,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -1369,10 +1436,10 @@
         <v>14.95</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="H14" s="8">
         <v>0</v>
@@ -1387,22 +1454,22 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
         <v>42</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>43</v>
-      </c>
-      <c r="D15" t="s">
-        <v>44</v>
       </c>
       <c r="E15" s="3">
         <v>19.95</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="H15" s="8">
         <v>0</v>
@@ -1417,7 +1484,7 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
@@ -1429,10 +1496,10 @@
         <v>4.95</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H16" s="8">
         <v>1</v>
@@ -1444,7 +1511,7 @@
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -1456,10 +1523,10 @@
         <v>1.95</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="H17" s="8">
         <v>1</v>
@@ -1474,7 +1541,7 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
@@ -1486,7 +1553,7 @@
         <v>2.95</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H18" s="8">
         <v>1</v>
@@ -1497,22 +1564,172 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="9"/>
+      <c r="A19">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>2030</v>
+      </c>
+      <c r="E19" s="3">
+        <v>14.95</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="H19" s="8">
+        <v>1</v>
+      </c>
+      <c r="I19" s="5">
+        <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Qty]]</f>
+        <v>14.95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" s="3">
+        <v>6.28</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H20" s="8">
+        <v>1</v>
+      </c>
+      <c r="I20" s="5">
+        <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Qty]]</f>
+        <v>6.28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" t="s">
+        <v>107</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H21" s="8">
+        <v>5</v>
+      </c>
+      <c r="I21" s="5">
+        <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Qty]]</f>
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>4007</v>
+      </c>
+      <c r="E22" s="3">
+        <v>3.95</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H22" s="8">
+        <v>2</v>
+      </c>
+      <c r="I22" s="5">
+        <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Qty]]</f>
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>18</v>
+      </c>
+      <c r="B23" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>3387</v>
+      </c>
+      <c r="E23" s="3">
+        <v>14.95</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H23" s="8">
+        <v>2</v>
+      </c>
+      <c r="I23" s="5">
+        <f>Table1[[#This Row],[Price/unit]]*Table1[[#This Row],[Qty]]</f>
+        <v>29.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="8">
         <f>SUBTOTAL(109,Table1[Qty])</f>
-        <v>30</v>
-      </c>
-      <c r="I19" s="10">
+        <v>32</v>
+      </c>
+      <c r="I24" s="10">
         <f>SUBTOTAL(109,Table1[Part Cost])</f>
-        <v>116.35000000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D22" s="5"/>
+        <v>151.88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D27" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1529,16 +1746,33 @@
     <hyperlink ref="G9" r:id="rId11" xr:uid="{029EF012-7656-4DA8-BCAA-FD947EB1E3B1}"/>
     <hyperlink ref="G10" r:id="rId12" xr:uid="{6B31B7D0-E1D2-4E46-8059-39B42325A4C4}"/>
     <hyperlink ref="G17" r:id="rId13" xr:uid="{8963FAFF-6DA0-4143-B175-33E66761586D}"/>
+    <hyperlink ref="G19" r:id="rId14" xr:uid="{AF2239AD-C237-4700-A9A9-C4CA73353D56}"/>
+    <hyperlink ref="G20" r:id="rId15" xr:uid="{A4DE5EB4-96A6-4771-9B41-C9FACBCAF4E2}"/>
+    <hyperlink ref="G21" r:id="rId16" xr:uid="{670C4A7A-E726-4BAB-B3AE-17EFD1860154}"/>
+    <hyperlink ref="G22" r:id="rId17" xr:uid="{073B2BB4-EF62-41B4-B016-9C528B1A42D5}"/>
+    <hyperlink ref="G23" r:id="rId18" xr:uid="{3519FA9B-6E9F-4AAA-9824-823364B7645E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
   <tableParts count="1">
-    <tablePart r:id="rId15"/>
+    <tablePart r:id="rId20"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E10FEBAD-DC72-40CF-9241-2BC96193365F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633AA69F-6F49-488D-9A1C-5AA8D7120116}">
   <dimension ref="A1:I7"/>
   <sheetViews>
@@ -1558,12 +1792,12 @@
   <sheetData>
     <row r="1" spans="1:9" ht="105" x14ac:dyDescent="0.35">
       <c r="B1" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -1584,10 +1818,10 @@
         <v>3</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1595,7 +1829,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -1607,10 +1841,10 @@
         <v>1.95</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="H3" s="12">
         <v>2</v>
@@ -1625,7 +1859,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -1637,10 +1871,10 @@
         <v>2.5</v>
       </c>
       <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="H4" s="12">
         <v>4</v>
@@ -1655,7 +1889,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1667,10 +1901,10 @@
         <v>1.5</v>
       </c>
       <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="H5" s="12">
         <v>4</v>
@@ -1685,7 +1919,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1697,10 +1931,10 @@
         <v>2.95</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H6" s="12">
         <v>5</v>
@@ -1712,7 +1946,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="11">
@@ -1738,11 +1972,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E71F0255-F518-4C33-8379-619E3ECE9F60}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -1759,12 +1993,12 @@
   <sheetData>
     <row r="1" spans="1:10" ht="105" x14ac:dyDescent="0.35">
       <c r="B1" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -1782,16 +2016,16 @@
         <v>2</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1799,10 +2033,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D3">
         <v>62179</v>
@@ -1811,13 +2045,13 @@
         <v>1.28</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="I3" s="12">
         <v>1</v>
@@ -1832,10 +2066,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D4">
         <v>491323</v>
@@ -1844,13 +2078,13 @@
         <v>1.28</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="G4" t="s">
-        <v>75</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="I4" s="12">
         <v>1</v>
@@ -1865,10 +2099,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" t="s">
         <v>93</v>
-      </c>
-      <c r="C5" t="s">
-        <v>94</v>
       </c>
       <c r="D5">
         <v>804271</v>
@@ -1877,13 +2111,13 @@
         <v>1.18</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I5" s="12">
         <v>1</v>
@@ -1898,10 +2132,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D6">
         <v>884489</v>
@@ -1910,13 +2144,13 @@
         <v>1.87</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I6" s="12">
         <v>2</v>
@@ -1931,10 +2165,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D7">
         <v>55844</v>
@@ -1943,13 +2177,13 @@
         <v>3.98</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="I7" s="12">
         <v>2</v>
@@ -1961,7 +2195,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="11">
@@ -1975,17 +2209,17 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>